<commit_message>
Update to cell size
</commit_message>
<xml_diff>
--- a/debate_flows1.xlsx
+++ b/debate_flows1.xlsx
@@ -14,27 +14,30 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="7">
-  <si>
-    <t>Contention 1: help me</t>
-  </si>
-  <si>
-    <t>Subpoint a: realy need it</t>
-  </si>
-  <si>
-    <t>Evidence (me): me</t>
-  </si>
-  <si>
-    <t>Contention 2: need help</t>
-  </si>
-  <si>
-    <t>Subpoint a: need help</t>
-  </si>
-  <si>
-    <t>Subpoint b: need help</t>
-  </si>
-  <si>
-    <t>Comments: need help</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="8">
+  <si>
+    <t>Contention 1: BUSH DID 9/11</t>
+  </si>
+  <si>
+    <t>Subpoint a: JET FUEL CAN'T MELT STEEL BEAMS</t>
+  </si>
+  <si>
+    <t>Evidence (your mother): JET FUEL CANT MELT STEEL BEAMS</t>
+  </si>
+  <si>
+    <t>Subpoint b: open your eyes sheeple</t>
+  </si>
+  <si>
+    <t>Evidence (trump): open</t>
+  </si>
+  <si>
+    <t>Contention 2: something really important</t>
+  </si>
+  <si>
+    <t>Subpoint a: jdafn</t>
+  </si>
+  <si>
+    <t>Subpoint b: jasdfn</t>
   </si>
 </sst>
 </file>
@@ -370,47 +373,62 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A13"/>
+  <dimension ref="A1:A15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelCol="0"/>
+  <cols>
+    <col customWidth="1" max="1" min="1" width="54"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
+    <row r="2" spans="1:1"/>
     <row r="3" spans="1:1">
       <c r="A3" t="s">
         <v>1</v>
       </c>
     </row>
+    <row r="4" spans="1:1"/>
     <row r="5" spans="1:1">
       <c r="A5" t="s">
         <v>2</v>
       </c>
     </row>
+    <row r="6" spans="1:1"/>
     <row r="7" spans="1:1">
       <c r="A7" t="s">
         <v>3</v>
       </c>
     </row>
+    <row r="8" spans="1:1"/>
     <row r="9" spans="1:1">
       <c r="A9" t="s">
         <v>4</v>
       </c>
     </row>
+    <row r="10" spans="1:1"/>
     <row r="11" spans="1:1">
       <c r="A11" t="s">
         <v>5</v>
       </c>
     </row>
+    <row r="12" spans="1:1"/>
     <row r="13" spans="1:1">
       <c r="A13" t="s">
         <v>6</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1"/>
+    <row r="15" spans="1:1">
+      <c r="A15" t="s">
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>